<commit_message>
Add Forms O and P
</commit_message>
<xml_diff>
--- a/xlsx/form_n_devolucao.xlsx
+++ b/xlsx/form_n_devolucao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Terra_Share\projects\CaVaTeCo_Collect\projects\monitor_forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Terra_Share\projects\CaVaTeCo_Collect\projects\odk_forms_cesc_niassa\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAF7442-676C-4A38-A8E2-034FDEE2729E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62BF734-A058-4207-A3C4-E44F1AAB410B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -914,9 +914,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1174,412 +1181,413 @@
   </borders>
   <cellStyleXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="243"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="243" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="243" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="242" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="243"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="243" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="243" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="243" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="242" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="243" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="243" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="244">
@@ -2165,11 +2173,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S124"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C92" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L109" sqref="L109"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2379,7 @@
       <c r="J13" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="70" t="s">
+      <c r="L13" s="80" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4181,7 +4189,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9187,8 +9195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>